<commit_message>
change test.py to direct to csv
</commit_message>
<xml_diff>
--- a/excel/model.xlsx
+++ b/excel/model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiddenpants-H\PycharmProjects\Antioxidant Protein Binary classification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A307F5-F39B-442B-B874-D9DB18B8C5F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F609602-B7FF-4FD1-AF1F-3F7D8596A322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DE2633A-700B-4BFF-9EE5-66DB1F5232EB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="15">
   <si>
     <t>model</t>
   </si>
@@ -84,10 +84,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -161,14 +168,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -178,8 +206,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C406722F-D0D7-4218-8B8E-A681B8557960}">
   <dimension ref="A1:AB129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55:J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,56 +542,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="6">
+      <c r="A1" s="3">
         <v>2538</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="L1" s="3" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="5"/>
-      <c r="R1" s="3" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="6"/>
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="5"/>
-      <c r="X1" s="3" t="s">
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="6"/>
+      <c r="X1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="5"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="6"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
@@ -635,65 +669,65 @@
       <c r="E3" s="1">
         <v>142</v>
       </c>
-      <c r="F3" s="1">
-        <v>0.98648650000000004</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.83673470000000005</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.86051500000000003</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.66041539999999999</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.91161060000000005</v>
+      <c r="F3" s="7">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.93700000000000006</v>
       </c>
       <c r="L3" s="1">
-        <v>0.97297299999999998</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="M3" s="1">
-        <v>0.92346936000000002</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="N3" s="1">
-        <v>0.93133043999999998</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="O3" s="1">
-        <v>0.79237449999999998</v>
+        <v>0.81299999999999994</v>
       </c>
       <c r="P3" s="1">
-        <v>0.94822114999999996</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="R3" s="1">
-        <v>0.98648650000000004</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="S3" s="1">
-        <v>0.91326529999999995</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="T3" s="1">
-        <v>0.92489270000000001</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="U3" s="1">
-        <v>0.78188429999999998</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="V3" s="1">
-        <v>0.94987582999999998</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="X3" s="2">
-        <v>0.98648650000000004</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="Y3" s="2">
-        <v>0.90816324999999998</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="Z3" s="2">
-        <v>0.92060083000000004</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="AA3" s="2">
-        <v>0.77243965999999997</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="AB3" s="2">
-        <v>0.94732490000000003</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -712,20 +746,20 @@
       <c r="E4" s="1">
         <v>142</v>
       </c>
-      <c r="F4" s="1">
-        <v>0.98648650000000004</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.90051020000000004</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.91416310000000001</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.75870029999999999</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.94349830000000001</v>
+      <c r="F4" s="8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -744,20 +778,20 @@
       <c r="E5" s="1">
         <v>142</v>
       </c>
-      <c r="F5" s="1">
-        <v>0.97297299999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.81377553999999996</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.83905580000000002</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.62109535999999999</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.98337430000000003</v>
+      <c r="F5" s="8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.91200000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -776,20 +810,20 @@
       <c r="E6" s="1">
         <v>142</v>
       </c>
-      <c r="F6" s="1">
-        <v>0.91891889999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.92602039999999997</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.92489270000000001</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.76065090000000002</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.9224696</v>
+      <c r="F6" s="8">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.93200000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -808,20 +842,20 @@
       <c r="E7" s="1">
         <v>142</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.98648650000000004</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.85969390000000001</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.87982833000000005</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.69288079999999996</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.92309015999999999</v>
+      <c r="F7" s="8">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.95799999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -840,20 +874,20 @@
       <c r="E8" s="1">
         <v>142</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.95945950000000002</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.86479589999999995</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.87982833000000005</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.68170549999999996</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.91212773000000003</v>
+      <c r="F8" s="8">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.93500000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -872,20 +906,20 @@
       <c r="E9" s="1">
         <v>141</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.95945950000000002</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.89795919999999996</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.90772533</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.73565835000000002</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0.92870940000000002</v>
+      <c r="F9" s="8">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -904,20 +938,20 @@
       <c r="E10" s="1">
         <v>141</v>
       </c>
-      <c r="F10" s="1">
-        <v>0.97297299999999998</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.88265305999999999</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.89699569999999995</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.7191381</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.92781305000000003</v>
+      <c r="F10" s="8">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.92800000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -936,23 +970,23 @@
       <c r="E11" s="1">
         <v>142</v>
       </c>
-      <c r="F11" s="1">
-        <v>0.93243240000000005</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.92091835</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.92274679999999998</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.75970674000000005</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0.92667529999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F11" s="8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -968,73 +1002,73 @@
       <c r="E12" s="1">
         <v>142</v>
       </c>
-      <c r="F12" s="1">
-        <v>0.85135139999999998</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.96173470000000005</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.94420599999999999</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0.7960351</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0.90654310000000005</v>
+      <c r="F12" s="9">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.86</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.91100000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>3128</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="1"/>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="5"/>
-      <c r="R14" s="3" t="s">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="6"/>
+      <c r="R14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="5"/>
-      <c r="X14" s="3" t="s">
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="6"/>
+      <c r="X14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="5"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="6"/>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1112,26 +1146,66 @@
       <c r="E16" s="1">
         <v>142</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
+      <c r="F16" s="7">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.86</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>0.94699999999999995</v>
+      </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1149,11 +1223,21 @@
       <c r="E17" s="1">
         <v>142</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="F17" s="8">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.94299999999999995</v>
+      </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1171,11 +1255,21 @@
       <c r="E18" s="1">
         <v>142</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="F18" s="8">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.621</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.98299999999999998</v>
+      </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1193,11 +1287,21 @@
       <c r="E19" s="1">
         <v>142</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="F19" s="8">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.92200000000000004</v>
+      </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1215,11 +1319,21 @@
       <c r="E20" s="1">
         <v>142</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="F20" s="8">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.92300000000000004</v>
+      </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1237,11 +1351,21 @@
       <c r="E21" s="1">
         <v>142</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="F21" s="8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0.91200000000000003</v>
+      </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -1259,11 +1383,21 @@
       <c r="E22" s="1">
         <v>141</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="F22" s="8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.92800000000000005</v>
+      </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1281,11 +1415,21 @@
       <c r="E23" s="1">
         <v>141</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="F23" s="8">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="J23" s="8">
+        <v>0.92700000000000005</v>
+      </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1303,13 +1447,23 @@
       <c r="E24" s="1">
         <v>142</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F24" s="8">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>9</v>
       </c>
@@ -1325,63 +1479,73 @@
       <c r="E25" s="1">
         <v>142</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="F25" s="9">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.90600000000000003</v>
+      </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="3">
+        <v>6210</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="1"/>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="5"/>
-      <c r="R27" s="3" t="s">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="6"/>
+      <c r="R27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="5"/>
-      <c r="X27" s="3" t="s">
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="6"/>
+      <c r="X27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
-      <c r="AB27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="6"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1459,26 +1623,66 @@
       <c r="E29" s="1">
         <v>142</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-      <c r="AA29" s="2"/>
-      <c r="AB29" s="2"/>
+      <c r="F29" s="1">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="X29" s="2">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="Z29" s="2">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>0.94499999999999995</v>
+      </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1496,11 +1700,21 @@
       <c r="E30" s="1">
         <v>142</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="F30" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.91600000000000004</v>
+      </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1518,11 +1732,21 @@
       <c r="E31" s="1">
         <v>142</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="F31" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.90800000000000003</v>
+      </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -1540,11 +1764,21 @@
       <c r="E32" s="1">
         <v>142</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="F32" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.94499999999999995</v>
+      </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -1562,11 +1796,21 @@
       <c r="E33" s="1">
         <v>142</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="F33" s="1">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.93400000000000005</v>
+      </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -1584,11 +1828,21 @@
       <c r="E34" s="1">
         <v>142</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="F34" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.879</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.91700000000000004</v>
+      </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -1606,11 +1860,21 @@
       <c r="E35" s="1">
         <v>141</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="F35" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.92900000000000005</v>
+      </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1628,11 +1892,21 @@
       <c r="E36" s="1">
         <v>141</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="F36" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.872</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.92200000000000004</v>
+      </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -1650,11 +1924,21 @@
       <c r="E37" s="1">
         <v>142</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="F37" s="1">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.95399999999999996</v>
+      </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -1672,63 +1956,73 @@
       <c r="E38" s="1">
         <v>142</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="F38" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="3">
+        <v>6233</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
       <c r="J40" s="1"/>
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="5"/>
-      <c r="R40" s="3" t="s">
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="6"/>
+      <c r="R40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="5"/>
-      <c r="X40" s="3" t="s">
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="6"/>
+      <c r="X40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
-      <c r="AA40" s="4"/>
-      <c r="AB40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="6"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
       <c r="F41" s="1" t="s">
         <v>6</v>
       </c>
@@ -1806,26 +2100,66 @@
       <c r="E42" s="1">
         <v>142</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="X42" s="2"/>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-      <c r="AA42" s="2"/>
-      <c r="AB42" s="2"/>
+      <c r="F42">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G42">
+        <v>0.88</v>
+      </c>
+      <c r="H42">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I42">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="J42">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="L42">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="M42">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="N42">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="O42">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="P42">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="R42">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="S42">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="T42">
+        <v>0.92</v>
+      </c>
+      <c r="U42">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="V42">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="X42">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="Y42">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="Z42">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AA42">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="AB42">
+        <v>0.95099999999999996</v>
+      </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -1843,11 +2177,21 @@
       <c r="E43" s="1">
         <v>142</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="F43">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G43">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="H43">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="I43">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="J43">
+        <v>0.94</v>
+      </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -1865,11 +2209,21 @@
       <c r="E44" s="1">
         <v>142</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="F44">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G44">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H44">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="I44">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J44">
+        <v>0.93500000000000005</v>
+      </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
@@ -1887,11 +2241,21 @@
       <c r="E45" s="1">
         <v>142</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="F45">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G45">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="H45">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="I45">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="J45">
+        <v>0.91200000000000003</v>
+      </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -1909,11 +2273,21 @@
       <c r="E46" s="1">
         <v>142</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
+      <c r="F46">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G46">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H46">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I46">
+        <v>0.7</v>
+      </c>
+      <c r="J46">
+        <v>0.92500000000000004</v>
+      </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -1931,11 +2305,21 @@
       <c r="E47" s="1">
         <v>142</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
+      <c r="F47">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="H47">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="I47">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="J47">
+        <v>0.92800000000000005</v>
+      </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -1953,11 +2337,21 @@
       <c r="E48" s="1">
         <v>141</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
+      <c r="F48">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G48">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="H48">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="I48">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="J48">
+        <v>0.91</v>
+      </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -1975,11 +2369,21 @@
       <c r="E49" s="1">
         <v>141</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
+      <c r="F49">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="G49">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="H49">
+        <v>0.871</v>
+      </c>
+      <c r="I49">
+        <v>0.66</v>
+      </c>
+      <c r="J49">
+        <v>0.90100000000000002</v>
+      </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -1997,11 +2401,21 @@
       <c r="E50" s="1">
         <v>142</v>
       </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="F50">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="G50">
+        <v>0.89</v>
+      </c>
+      <c r="H50">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="I50">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="J50">
+        <v>0.91100000000000003</v>
+      </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -2019,63 +2433,73 @@
       <c r="E51" s="1">
         <v>142</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
+      <c r="F51">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G51">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="H51">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="I51">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="J51">
+        <v>0.92700000000000005</v>
+      </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="3">
+        <v>8730</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
       <c r="J53" s="1"/>
-      <c r="L53" s="3" t="s">
+      <c r="L53" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="5"/>
-      <c r="R53" s="3" t="s">
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="6"/>
+      <c r="R53" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
-      <c r="V53" s="5"/>
-      <c r="X53" s="3" t="s">
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="6"/>
+      <c r="X53" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y53" s="4"/>
-      <c r="Z53" s="4"/>
-      <c r="AA53" s="4"/>
-      <c r="AB53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="6"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
       <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
@@ -2153,26 +2577,66 @@
       <c r="E55" s="1">
         <v>142</v>
       </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="X55" s="2"/>
-      <c r="Y55" s="2"/>
-      <c r="Z55" s="2"/>
-      <c r="AA55" s="2"/>
-      <c r="AB55" s="2"/>
+      <c r="F55">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G55">
+        <v>0.877</v>
+      </c>
+      <c r="H55">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I55">
+        <v>0.71</v>
+      </c>
+      <c r="J55">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="L55">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="M55">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="N55">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="O55">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="P55">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="R55">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="S55">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="T55">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="U55">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="V55">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="X55">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="Y55">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="Z55">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AA55">
+        <v>0.754</v>
+      </c>
+      <c r="AB55">
+        <v>0.94199999999999995</v>
+      </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
@@ -2190,11 +2654,21 @@
       <c r="E56" s="1">
         <v>142</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
+      <c r="F56">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G56">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="H56">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="I56">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="J56">
+        <v>0.92400000000000004</v>
+      </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
@@ -2212,11 +2686,21 @@
       <c r="E57" s="1">
         <v>142</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
+      <c r="F57">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G57">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="H57">
+        <v>0.875</v>
+      </c>
+      <c r="I57">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="J57">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
@@ -2234,11 +2718,21 @@
       <c r="E58" s="1">
         <v>142</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
+      <c r="F58">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G58">
+        <v>0.875</v>
+      </c>
+      <c r="H58">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I58">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="J58">
+        <v>0.93</v>
+      </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -2256,11 +2750,21 @@
       <c r="E59" s="1">
         <v>142</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
+      <c r="F59">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G59">
+        <v>0.89</v>
+      </c>
+      <c r="H59">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="I59">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="J59">
+        <v>0.93100000000000005</v>
+      </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -2278,11 +2782,21 @@
       <c r="E60" s="1">
         <v>142</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
+      <c r="F60">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="G60">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="H60">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="I60">
+        <v>0.754</v>
+      </c>
+      <c r="J60">
+        <v>0.92900000000000005</v>
+      </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -2300,11 +2814,21 @@
       <c r="E61" s="1">
         <v>141</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
+      <c r="F61">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="G61">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H61">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I61">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="J61">
+        <v>0.93600000000000005</v>
+      </c>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -2322,11 +2846,21 @@
       <c r="E62" s="1">
         <v>141</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
+      <c r="F62">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G62">
+        <v>0.88</v>
+      </c>
+      <c r="H62">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I62">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="J62">
+        <v>0.91900000000000004</v>
+      </c>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -2344,11 +2878,21 @@
       <c r="E63" s="1">
         <v>142</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
+      <c r="F63">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G63">
+        <v>0.88</v>
+      </c>
+      <c r="H63">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="I63">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="J63">
+        <v>0.92600000000000005</v>
+      </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
@@ -2366,63 +2910,73 @@
       <c r="E64" s="1">
         <v>142</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
+      <c r="F64">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G64">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H64">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I64">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="J64">
+        <v>0.90200000000000002</v>
+      </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E66" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F66" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
       <c r="J66" s="1"/>
-      <c r="L66" s="3" t="s">
+      <c r="L66" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="5"/>
-      <c r="R66" s="3" t="s">
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="6"/>
+      <c r="R66" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4"/>
-      <c r="V66" s="5"/>
-      <c r="X66" s="3" t="s">
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="6"/>
+      <c r="X66" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y66" s="4"/>
-      <c r="Z66" s="4"/>
-      <c r="AA66" s="4"/>
-      <c r="AB66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+      <c r="AA66" s="5"/>
+      <c r="AB66" s="6"/>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
       <c r="F67" s="1" t="s">
         <v>6</v>
       </c>
@@ -2720,56 +3274,56 @@
       <c r="J77" s="1"/>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F79" s="6" t="s">
+      <c r="F79" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
       <c r="J79" s="1"/>
-      <c r="L79" s="3" t="s">
+      <c r="L79" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="5"/>
-      <c r="R79" s="3" t="s">
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="6"/>
+      <c r="R79" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S79" s="4"/>
-      <c r="T79" s="4"/>
-      <c r="U79" s="4"/>
-      <c r="V79" s="5"/>
-      <c r="X79" s="3" t="s">
+      <c r="S79" s="5"/>
+      <c r="T79" s="5"/>
+      <c r="U79" s="5"/>
+      <c r="V79" s="6"/>
+      <c r="X79" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y79" s="4"/>
-      <c r="Z79" s="4"/>
-      <c r="AA79" s="4"/>
-      <c r="AB79" s="5"/>
+      <c r="Y79" s="5"/>
+      <c r="Z79" s="5"/>
+      <c r="AA79" s="5"/>
+      <c r="AB79" s="6"/>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
       <c r="F80" s="1" t="s">
         <v>6</v>
       </c>
@@ -3067,56 +3621,56 @@
       <c r="J90" s="1"/>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="D92" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E92" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F92" s="6" t="s">
+      <c r="F92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
       <c r="J92" s="1"/>
-      <c r="L92" s="3" t="s">
+      <c r="L92" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="5"/>
-      <c r="R92" s="3" t="s">
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="6"/>
+      <c r="R92" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S92" s="4"/>
-      <c r="T92" s="4"/>
-      <c r="U92" s="4"/>
-      <c r="V92" s="5"/>
-      <c r="X92" s="3" t="s">
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="5"/>
+      <c r="V92" s="6"/>
+      <c r="X92" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y92" s="4"/>
-      <c r="Z92" s="4"/>
-      <c r="AA92" s="4"/>
-      <c r="AB92" s="5"/>
+      <c r="Y92" s="5"/>
+      <c r="Z92" s="5"/>
+      <c r="AA92" s="5"/>
+      <c r="AB92" s="6"/>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
       <c r="F93" s="1" t="s">
         <v>6</v>
       </c>
@@ -3414,56 +3968,56 @@
       <c r="J103" s="1"/>
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="C105" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D105" s="6" t="s">
+      <c r="D105" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E105" s="6" t="s">
+      <c r="E105" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F105" s="6" t="s">
+      <c r="F105" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="6"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
       <c r="J105" s="1"/>
-      <c r="L105" s="3" t="s">
+      <c r="L105" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="5"/>
-      <c r="R105" s="3" t="s">
+      <c r="M105" s="5"/>
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="6"/>
+      <c r="R105" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S105" s="4"/>
-      <c r="T105" s="4"/>
-      <c r="U105" s="4"/>
-      <c r="V105" s="5"/>
-      <c r="X105" s="3" t="s">
+      <c r="S105" s="5"/>
+      <c r="T105" s="5"/>
+      <c r="U105" s="5"/>
+      <c r="V105" s="6"/>
+      <c r="X105" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y105" s="4"/>
-      <c r="Z105" s="4"/>
-      <c r="AA105" s="4"/>
-      <c r="AB105" s="5"/>
+      <c r="Y105" s="5"/>
+      <c r="Z105" s="5"/>
+      <c r="AA105" s="5"/>
+      <c r="AB105" s="6"/>
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
       <c r="F106" s="1" t="s">
         <v>6</v>
       </c>
@@ -3761,56 +4315,56 @@
       <c r="J116" s="1"/>
     </row>
     <row r="118" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A118" s="6" t="s">
+      <c r="A118" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B118" s="6" t="s">
+      <c r="B118" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C118" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D118" s="6" t="s">
+      <c r="D118" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E118" s="6" t="s">
+      <c r="E118" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F118" s="6" t="s">
+      <c r="F118" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G118" s="6"/>
-      <c r="H118" s="6"/>
-      <c r="I118" s="6"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
       <c r="J118" s="1"/>
-      <c r="L118" s="3" t="s">
+      <c r="L118" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M118" s="4"/>
-      <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="5"/>
-      <c r="R118" s="3" t="s">
+      <c r="M118" s="5"/>
+      <c r="N118" s="5"/>
+      <c r="O118" s="5"/>
+      <c r="P118" s="6"/>
+      <c r="R118" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S118" s="4"/>
-      <c r="T118" s="4"/>
-      <c r="U118" s="4"/>
-      <c r="V118" s="5"/>
-      <c r="X118" s="3" t="s">
+      <c r="S118" s="5"/>
+      <c r="T118" s="5"/>
+      <c r="U118" s="5"/>
+      <c r="V118" s="6"/>
+      <c r="X118" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y118" s="4"/>
-      <c r="Z118" s="4"/>
-      <c r="AA118" s="4"/>
-      <c r="AB118" s="5"/>
+      <c r="Y118" s="5"/>
+      <c r="Z118" s="5"/>
+      <c r="AA118" s="5"/>
+      <c r="AB118" s="6"/>
     </row>
     <row r="119" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A119" s="6"/>
-      <c r="B119" s="6"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
       <c r="F119" s="1" t="s">
         <v>6</v>
       </c>
@@ -4109,53 +4663,33 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F118:I118"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="L118:P118"/>
+    <mergeCell ref="R118:V118"/>
+    <mergeCell ref="X118:AB118"/>
+    <mergeCell ref="L92:P92"/>
+    <mergeCell ref="R92:V92"/>
+    <mergeCell ref="X92:AB92"/>
+    <mergeCell ref="L105:P105"/>
+    <mergeCell ref="R105:V105"/>
+    <mergeCell ref="X105:AB105"/>
+    <mergeCell ref="L66:P66"/>
+    <mergeCell ref="R66:V66"/>
+    <mergeCell ref="X66:AB66"/>
+    <mergeCell ref="L79:P79"/>
+    <mergeCell ref="R79:V79"/>
+    <mergeCell ref="X79:AB79"/>
+    <mergeCell ref="L40:P40"/>
+    <mergeCell ref="R40:V40"/>
+    <mergeCell ref="X40:AB40"/>
+    <mergeCell ref="L53:P53"/>
+    <mergeCell ref="R53:V53"/>
+    <mergeCell ref="X53:AB53"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="L27:P27"/>
+    <mergeCell ref="R27:V27"/>
+    <mergeCell ref="X27:AB27"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="R1:V1"/>
@@ -4172,34 +4706,55 @@
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="R14:V14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="L27:P27"/>
-    <mergeCell ref="R27:V27"/>
-    <mergeCell ref="X27:AB27"/>
-    <mergeCell ref="L40:P40"/>
-    <mergeCell ref="R40:V40"/>
-    <mergeCell ref="X40:AB40"/>
-    <mergeCell ref="L53:P53"/>
-    <mergeCell ref="R53:V53"/>
-    <mergeCell ref="X53:AB53"/>
-    <mergeCell ref="L66:P66"/>
-    <mergeCell ref="R66:V66"/>
-    <mergeCell ref="X66:AB66"/>
-    <mergeCell ref="L79:P79"/>
-    <mergeCell ref="R79:V79"/>
-    <mergeCell ref="X79:AB79"/>
-    <mergeCell ref="L118:P118"/>
-    <mergeCell ref="R118:V118"/>
-    <mergeCell ref="X118:AB118"/>
-    <mergeCell ref="L92:P92"/>
-    <mergeCell ref="R92:V92"/>
-    <mergeCell ref="X92:AB92"/>
-    <mergeCell ref="L105:P105"/>
-    <mergeCell ref="R105:V105"/>
-    <mergeCell ref="X105:AB105"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F118:I118"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>